<commit_message>
Updated SQ9 (added automatic transitions based on data from 2K pumps system). Updated opi and documentation.
</commit_message>
<xml_diff>
--- a/doc/EPICS_dialog_V133.xlsx
+++ b/doc/EPICS_dialog_V133.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18690" windowHeight="10050" tabRatio="595" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18690" windowHeight="10050" tabRatio="595"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,14 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
-    <customWorkbookView name="Konrad Gajewski - Personal View" guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" mergeInterval="0" personalView="1" xWindow="72" yWindow="55" windowWidth="2807" windowHeight="1299" tabRatio="595" activeSheetId="3"/>
+    <customWorkbookView name="Konrad Gajewski - Personal View" guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" mergeInterval="0" personalView="1" xWindow="72" yWindow="55" windowWidth="2580" windowHeight="1299" tabRatio="595" activeSheetId="4"/>
     <customWorkbookView name="Adrien JOURNIAT - Affichage personnalisé" guid="{0FB11559-FF5E-4B68-9C91-951C6118F018}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="855" tabRatio="595" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="1125">
   <si>
     <t>EPICS -&gt; PLC</t>
   </si>
@@ -3857,13 +3857,19 @@
     <t>Standard Cernox set connected to the cavities</t>
   </si>
   <si>
-    <t>Added extra bits in general parameters. Changed general parameter cParR16 to 32 boolean parameters. Added extra boolean parameter in SQ7 to automatically start SQ8</t>
-  </si>
-  <si>
     <t>Automatically start SQ8 when TRUE</t>
   </si>
   <si>
     <t>P_StartSQ8</t>
+  </si>
+  <si>
+    <t>PT552_2K_pumps</t>
+  </si>
+  <si>
+    <t>PT552 from 2K pumps (wtrvac IOC)</t>
+  </si>
+  <si>
+    <t>Added extra bits in general parameters. Changed general parameter cParR16 to 32 boolean parameters. Added extra boolean parameter in SQ7 to automatically start SQ8. Added new boolean parameters in SQ9 to automaticaly control 2K pumps by the sequencer program. Added Gen param for PT552 from 2K pumps</t>
   </si>
 </sst>
 </file>
@@ -4192,7 +4198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -4531,6 +4537,12 @@
     <xf numFmtId="0" fontId="5" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -4639,9 +4651,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4660,7 +4669,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{9E6879EC-C471-4F20-AA22-2E5858EB476B}" diskRevisions="1" revisionId="658" version="8">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{12DBE06C-2D7D-47B4-9499-6F913E13C6D3}" diskRevisions="1" revisionId="664" version="11">
   <header guid="{467B07E6-3486-485E-8865-6DC5865535AD}" dateTime="2025-01-23T13:50:35" maxSheetId="7" userName="Konrad Gajewski" r:id="rId49" minRId="304" maxRId="434">
     <sheetIdMap count="6">
       <sheetId val="1"/>
@@ -4722,6 +4731,36 @@
     </sheetIdMap>
   </header>
   <header guid="{9E6879EC-C471-4F20-AA22-2E5858EB476B}" dateTime="2025-01-30T10:41:50" maxSheetId="7" userName="Konrad Gajewski" r:id="rId55" minRId="655" maxRId="657">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{97C9943F-0957-40EC-8B6B-C3C16D7964A8}" dateTime="2025-01-30T10:50:59" maxSheetId="7" userName="Konrad Gajewski" r:id="rId56" minRId="659">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4185F9C0-A442-4C78-9E3F-615C30115450}" dateTime="2025-02-05T10:51:07" maxSheetId="7" userName="Konrad Gajewski" r:id="rId57" minRId="661" maxRId="662">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{12DBE06C-2D7D-47B4-9499-6F913E13C6D3}" dateTime="2025-02-05T10:52:46" maxSheetId="7" userName="Konrad Gajewski" r:id="rId58" minRId="664">
     <sheetIdMap count="6">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -5856,6 +5895,23 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="664" sId="1">
+    <oc r="C23" t="inlineStr">
+      <is>
+        <t>Added extra bits in general parameters. Changed general parameter cParR16 to 32 boolean parameters. Added extra boolean parameter in SQ7 to automatically start SQ8. Added new boolean parameters in SQ9 to automaticaly control 2K pumps by the sequencer program.</t>
+      </is>
+    </oc>
+    <nc r="C23" t="inlineStr">
+      <is>
+        <t>Added extra bits in general parameters. Changed general parameter cParR16 to 32 boolean parameters. Added extra boolean parameter in SQ7 to automatically start SQ8. Added new boolean parameters in SQ9 to automaticaly control 2K pumps by the sequencer program. Added Gen param for PT552 from 2K pumps</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="653" sId="4">
@@ -5939,6 +5995,94 @@
     </nc>
   </rcc>
   <rfmt sheetId="3" sqref="W18:X18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="65"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rcv guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" action="delete"/>
+  <rdn rId="0" localSheetId="3" customView="1" name="Z_707DC1D0_2077_4C17_8276_287DF75CEF77_.wvu.PrintArea" hidden="1" oldHidden="1">
+    <formula>Sequences!$B$54:$E$118</formula>
+    <oldFormula>Sequences!$B$54:$E$118</oldFormula>
+  </rdn>
+  <rcv guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="C1:C1048576">
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="659" sId="1">
+    <oc r="C23" t="inlineStr">
+      <is>
+        <t>Added extra bits in general parameters. Changed general parameter cParR16 to 32 boolean parameters. Added extra boolean parameter in SQ7 to automatically start SQ8</t>
+      </is>
+    </oc>
+    <nc r="C23" t="inlineStr">
+      <is>
+        <t>Added extra bits in general parameters. Changed general parameter cParR16 to 32 boolean parameters. Added extra boolean parameter in SQ7 to automatically start SQ8. Added new boolean parameters in SQ9 to automaticaly control 2K pumps by the sequencer program.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" action="delete"/>
+  <rdn rId="0" localSheetId="3" customView="1" name="Z_707DC1D0_2077_4C17_8276_287DF75CEF77_.wvu.PrintArea" hidden="1" oldHidden="1">
+    <formula>Sequences!$B$54:$E$118</formula>
+    <oldFormula>Sequences!$B$54:$E$118</oldFormula>
+  </rdn>
+  <rcv guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="661" sId="4">
+    <oc r="D40" t="inlineStr">
+      <is>
+        <t>cParR8</t>
+      </is>
+    </oc>
+    <nc r="D40" t="inlineStr">
+      <is>
+        <t>PT552_2K_pumps</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="662" sId="4">
+    <oc r="E40" t="inlineStr">
+      <is>
+        <t>Real - Dialogue</t>
+      </is>
+    </oc>
+    <nc r="E40" t="inlineStr">
+      <is>
+        <t>PT552 from 2K pumps (wtrvac IOC)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="4" sqref="B40:E40">
     <dxf>
       <font>
         <b val="0"/>
@@ -10363,13 +10507,13 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="102.85546875" style="127" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -10425,6 +10569,7 @@
         <v>894</v>
       </c>
       <c r="B9" s="55"/>
+      <c r="C9" s="127"/>
     </row>
     <row r="10" spans="1:3" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="53" t="s">
@@ -10433,6 +10578,7 @@
       <c r="B10" s="59">
         <v>42165</v>
       </c>
+      <c r="C10" s="127"/>
     </row>
     <row r="11" spans="1:3" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
@@ -10441,6 +10587,7 @@
       <c r="B11" s="59">
         <v>42245</v>
       </c>
+      <c r="C11" s="127"/>
     </row>
     <row r="12" spans="1:3" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
@@ -10449,7 +10596,7 @@
       <c r="B12" s="60">
         <v>42769</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="127" t="s">
         <v>921</v>
       </c>
     </row>
@@ -10460,7 +10607,7 @@
       <c r="B13" s="63">
         <v>43000</v>
       </c>
-      <c r="C13" s="53" t="s">
+      <c r="C13" s="127" t="s">
         <v>922</v>
       </c>
     </row>
@@ -10471,7 +10618,7 @@
       <c r="B14" s="69">
         <v>43126</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="127" t="s">
         <v>932</v>
       </c>
     </row>
@@ -10482,7 +10629,7 @@
       <c r="B15" s="73">
         <v>43259</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="127" t="s">
         <v>934</v>
       </c>
     </row>
@@ -10493,7 +10640,7 @@
       <c r="B16" s="77">
         <v>43332</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="127" t="s">
         <v>953</v>
       </c>
     </row>
@@ -10504,7 +10651,7 @@
       <c r="B17" s="83">
         <v>43419</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="127" t="s">
         <v>967</v>
       </c>
     </row>
@@ -10515,7 +10662,7 @@
       <c r="B18" s="84">
         <v>43424</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="127" t="s">
         <v>969</v>
       </c>
     </row>
@@ -10526,7 +10673,7 @@
       <c r="B19" s="88">
         <v>43587</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="127" t="s">
         <v>980</v>
       </c>
     </row>
@@ -10537,7 +10684,7 @@
       <c r="B20" s="93">
         <v>44173</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="127" t="s">
         <v>982</v>
       </c>
     </row>
@@ -10548,7 +10695,7 @@
       <c r="B21" s="98">
         <v>44285</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="127" t="s">
         <v>1003</v>
       </c>
     </row>
@@ -10559,25 +10706,25 @@
       <c r="B22" s="114">
         <v>45680</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="127" t="s">
         <v>1075</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="53" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
         <v>1081</v>
       </c>
       <c r="B23" s="122">
         <v>45687</v>
       </c>
-      <c r="C23" s="53" t="s">
-        <v>1120</v>
+      <c r="C23" s="127" t="s">
+        <v>1124</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D23" sqref="D23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -10646,75 +10793,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
     </row>
     <row r="2" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B2" s="135"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
     </row>
     <row r="3" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
-      <c r="I4" s="138"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="140"/>
       <c r="K4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="AT4" s="3"/>
     </row>
     <row r="5" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B5" s="129" t="s">
+      <c r="B5" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="129" t="s">
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="131"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="133"/>
       <c r="M5" s="1" t="s">
         <v>116</v>
       </c>
       <c r="AT5" s="3"/>
     </row>
     <row r="6" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="133"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="132" t="s">
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="134" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="133"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="134"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="136"/>
       <c r="K6" s="2" t="s">
         <v>114</v>
       </c>
@@ -10910,50 +11057,50 @@
     </row>
     <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="136" t="s">
+      <c r="B19" s="138" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="137"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="137"/>
-      <c r="F19" s="137"/>
-      <c r="G19" s="137"/>
-      <c r="H19" s="137"/>
-      <c r="I19" s="138"/>
+      <c r="C19" s="139"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="139"/>
+      <c r="I19" s="140"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="129" t="s">
+      <c r="B20" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="130"/>
-      <c r="D20" s="130"/>
-      <c r="E20" s="131"/>
-      <c r="F20" s="130" t="s">
+      <c r="C20" s="132"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="130"/>
-      <c r="H20" s="130"/>
-      <c r="I20" s="131"/>
+      <c r="G20" s="132"/>
+      <c r="H20" s="132"/>
+      <c r="I20" s="133"/>
       <c r="M20" s="4" t="s">
         <v>471</v>
       </c>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="132" t="s">
+      <c r="B21" s="134" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="133"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="134"/>
-      <c r="F21" s="133" t="s">
+      <c r="C21" s="135"/>
+      <c r="D21" s="135"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="135" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="133"/>
-      <c r="H21" s="133"/>
-      <c r="I21" s="134"/>
+      <c r="G21" s="135"/>
+      <c r="H21" s="135"/>
+      <c r="I21" s="136"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
@@ -11122,16 +11269,16 @@
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="136" t="s">
+      <c r="B31" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="137"/>
-      <c r="D31" s="137"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="137"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="137"/>
-      <c r="I31" s="138"/>
+      <c r="C31" s="139"/>
+      <c r="D31" s="139"/>
+      <c r="E31" s="139"/>
+      <c r="F31" s="139"/>
+      <c r="G31" s="139"/>
+      <c r="H31" s="139"/>
+      <c r="I31" s="140"/>
       <c r="K31" s="2" t="s">
         <v>41</v>
       </c>
@@ -11139,36 +11286,36 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="129" t="s">
+      <c r="B32" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="130"/>
-      <c r="D32" s="130"/>
-      <c r="E32" s="131"/>
-      <c r="F32" s="129" t="s">
+      <c r="C32" s="132"/>
+      <c r="D32" s="132"/>
+      <c r="E32" s="133"/>
+      <c r="F32" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="130"/>
-      <c r="H32" s="130"/>
-      <c r="I32" s="131"/>
+      <c r="G32" s="132"/>
+      <c r="H32" s="132"/>
+      <c r="I32" s="133"/>
       <c r="M32" s="4" t="s">
         <v>45</v>
       </c>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="132" t="s">
+      <c r="B33" s="134" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="133"/>
-      <c r="D33" s="133"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="132" t="s">
+      <c r="C33" s="135"/>
+      <c r="D33" s="135"/>
+      <c r="E33" s="136"/>
+      <c r="F33" s="134" t="s">
         <v>65</v>
       </c>
-      <c r="G33" s="133"/>
-      <c r="H33" s="133"/>
-      <c r="I33" s="134"/>
+      <c r="G33" s="135"/>
+      <c r="H33" s="135"/>
+      <c r="I33" s="136"/>
       <c r="K33" s="2" t="s">
         <v>42</v>
       </c>
@@ -11437,16 +11584,16 @@
     </row>
     <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="136" t="s">
+      <c r="B46" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="137"/>
-      <c r="D46" s="137"/>
-      <c r="E46" s="137"/>
-      <c r="F46" s="137"/>
-      <c r="G46" s="137"/>
-      <c r="H46" s="137"/>
-      <c r="I46" s="138"/>
+      <c r="C46" s="139"/>
+      <c r="D46" s="139"/>
+      <c r="E46" s="139"/>
+      <c r="F46" s="139"/>
+      <c r="G46" s="139"/>
+      <c r="H46" s="139"/>
+      <c r="I46" s="140"/>
       <c r="K46" s="2" t="s">
         <v>41</v>
       </c>
@@ -11454,36 +11601,36 @@
       <c r="N46" s="4"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="129" t="s">
+      <c r="B47" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="130"/>
-      <c r="D47" s="130"/>
-      <c r="E47" s="131"/>
-      <c r="F47" s="129" t="s">
+      <c r="C47" s="132"/>
+      <c r="D47" s="132"/>
+      <c r="E47" s="133"/>
+      <c r="F47" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="G47" s="130"/>
-      <c r="H47" s="130"/>
-      <c r="I47" s="131"/>
+      <c r="G47" s="132"/>
+      <c r="H47" s="132"/>
+      <c r="I47" s="133"/>
       <c r="M47" s="4" t="s">
         <v>45</v>
       </c>
       <c r="N47" s="4"/>
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="132" t="s">
+      <c r="B48" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="133"/>
-      <c r="D48" s="133"/>
-      <c r="E48" s="134"/>
-      <c r="F48" s="132" t="s">
+      <c r="C48" s="135"/>
+      <c r="D48" s="135"/>
+      <c r="E48" s="136"/>
+      <c r="F48" s="134" t="s">
         <v>75</v>
       </c>
-      <c r="G48" s="133"/>
-      <c r="H48" s="133"/>
-      <c r="I48" s="134"/>
+      <c r="G48" s="135"/>
+      <c r="H48" s="135"/>
+      <c r="I48" s="136"/>
       <c r="K48" s="2" t="s">
         <v>42</v>
       </c>
@@ -11706,16 +11853,16 @@
       <c r="I60" s="4"/>
     </row>
     <row r="61" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="136" t="s">
+      <c r="B61" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="137"/>
-      <c r="D61" s="137"/>
-      <c r="E61" s="137"/>
-      <c r="F61" s="137"/>
-      <c r="G61" s="137"/>
-      <c r="H61" s="137"/>
-      <c r="I61" s="138"/>
+      <c r="C61" s="139"/>
+      <c r="D61" s="139"/>
+      <c r="E61" s="139"/>
+      <c r="F61" s="139"/>
+      <c r="G61" s="139"/>
+      <c r="H61" s="139"/>
+      <c r="I61" s="140"/>
       <c r="K61" s="2" t="s">
         <v>41</v>
       </c>
@@ -11723,36 +11870,36 @@
       <c r="N61" s="4"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="129" t="s">
+      <c r="B62" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C62" s="130"/>
-      <c r="D62" s="130"/>
-      <c r="E62" s="131"/>
-      <c r="F62" s="130" t="s">
+      <c r="C62" s="132"/>
+      <c r="D62" s="132"/>
+      <c r="E62" s="133"/>
+      <c r="F62" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="G62" s="130"/>
-      <c r="H62" s="130"/>
-      <c r="I62" s="131"/>
+      <c r="G62" s="132"/>
+      <c r="H62" s="132"/>
+      <c r="I62" s="133"/>
       <c r="M62" s="4" t="s">
         <v>48</v>
       </c>
       <c r="N62" s="4"/>
     </row>
     <row r="63" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="126" t="s">
+      <c r="B63" s="128" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="127"/>
-      <c r="D63" s="127"/>
-      <c r="E63" s="128"/>
-      <c r="F63" s="127" t="s">
+      <c r="C63" s="129"/>
+      <c r="D63" s="129"/>
+      <c r="E63" s="130"/>
+      <c r="F63" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="G63" s="127"/>
-      <c r="H63" s="127"/>
-      <c r="I63" s="128"/>
+      <c r="G63" s="129"/>
+      <c r="H63" s="129"/>
+      <c r="I63" s="130"/>
       <c r="K63" s="2" t="s">
         <v>42</v>
       </c>
@@ -11917,16 +12064,16 @@
       <c r="AT72" s="3"/>
     </row>
     <row r="73" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="136" t="s">
+      <c r="B73" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="137"/>
-      <c r="D73" s="137"/>
-      <c r="E73" s="137"/>
-      <c r="F73" s="137"/>
-      <c r="G73" s="137"/>
-      <c r="H73" s="137"/>
-      <c r="I73" s="138"/>
+      <c r="C73" s="139"/>
+      <c r="D73" s="139"/>
+      <c r="E73" s="139"/>
+      <c r="F73" s="139"/>
+      <c r="G73" s="139"/>
+      <c r="H73" s="139"/>
+      <c r="I73" s="140"/>
       <c r="K73" s="2" t="s">
         <v>145</v>
       </c>
@@ -11935,36 +12082,36 @@
       <c r="AT73" s="3"/>
     </row>
     <row r="74" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B74" s="129" t="s">
+      <c r="B74" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C74" s="130"/>
-      <c r="D74" s="130"/>
-      <c r="E74" s="131"/>
-      <c r="F74" s="130" t="s">
+      <c r="C74" s="132"/>
+      <c r="D74" s="132"/>
+      <c r="E74" s="133"/>
+      <c r="F74" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="G74" s="130"/>
-      <c r="H74" s="130"/>
-      <c r="I74" s="131"/>
+      <c r="G74" s="132"/>
+      <c r="H74" s="132"/>
+      <c r="I74" s="133"/>
       <c r="M74" s="1" t="s">
         <v>50</v>
       </c>
       <c r="AT74" s="3"/>
     </row>
     <row r="75" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="132" t="s">
+      <c r="B75" s="134" t="s">
         <v>68</v>
       </c>
-      <c r="C75" s="133"/>
-      <c r="D75" s="133"/>
-      <c r="E75" s="134"/>
-      <c r="F75" s="133" t="s">
+      <c r="C75" s="135"/>
+      <c r="D75" s="135"/>
+      <c r="E75" s="136"/>
+      <c r="F75" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="G75" s="133"/>
-      <c r="H75" s="133"/>
-      <c r="I75" s="134"/>
+      <c r="G75" s="135"/>
+      <c r="H75" s="135"/>
+      <c r="I75" s="136"/>
       <c r="M75" s="4" t="s">
         <v>51</v>
       </c>
@@ -12294,16 +12441,16 @@
       <c r="AT89" s="3"/>
     </row>
     <row r="90" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="136" t="s">
+      <c r="B90" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="C90" s="137"/>
-      <c r="D90" s="137"/>
-      <c r="E90" s="137"/>
-      <c r="F90" s="137"/>
-      <c r="G90" s="137"/>
-      <c r="H90" s="137"/>
-      <c r="I90" s="138"/>
+      <c r="C90" s="139"/>
+      <c r="D90" s="139"/>
+      <c r="E90" s="139"/>
+      <c r="F90" s="139"/>
+      <c r="G90" s="139"/>
+      <c r="H90" s="139"/>
+      <c r="I90" s="140"/>
       <c r="K90" s="2" t="s">
         <v>41</v>
       </c>
@@ -12312,18 +12459,18 @@
       <c r="AT90" s="3"/>
     </row>
     <row r="91" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B91" s="129" t="s">
+      <c r="B91" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C91" s="130"/>
-      <c r="D91" s="130"/>
-      <c r="E91" s="131"/>
-      <c r="F91" s="130" t="s">
+      <c r="C91" s="132"/>
+      <c r="D91" s="132"/>
+      <c r="E91" s="133"/>
+      <c r="F91" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="G91" s="130"/>
-      <c r="H91" s="130"/>
-      <c r="I91" s="131"/>
+      <c r="G91" s="132"/>
+      <c r="H91" s="132"/>
+      <c r="I91" s="133"/>
       <c r="M91" s="4" t="s">
         <v>45</v>
       </c>
@@ -12331,18 +12478,18 @@
       <c r="AT91" s="3"/>
     </row>
     <row r="92" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="126" t="s">
+      <c r="B92" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="C92" s="127"/>
-      <c r="D92" s="127"/>
-      <c r="E92" s="128"/>
-      <c r="F92" s="127" t="s">
+      <c r="C92" s="129"/>
+      <c r="D92" s="129"/>
+      <c r="E92" s="130"/>
+      <c r="F92" s="129" t="s">
         <v>71</v>
       </c>
-      <c r="G92" s="127"/>
-      <c r="H92" s="127"/>
-      <c r="I92" s="128"/>
+      <c r="G92" s="129"/>
+      <c r="H92" s="129"/>
+      <c r="I92" s="130"/>
       <c r="K92" s="2" t="s">
         <v>42</v>
       </c>
@@ -12702,16 +12849,16 @@
       <c r="I112" s="4"/>
     </row>
     <row r="113" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="136" t="s">
+      <c r="B113" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="C113" s="137"/>
-      <c r="D113" s="137"/>
-      <c r="E113" s="137"/>
-      <c r="F113" s="137"/>
-      <c r="G113" s="137"/>
-      <c r="H113" s="137"/>
-      <c r="I113" s="138"/>
+      <c r="C113" s="139"/>
+      <c r="D113" s="139"/>
+      <c r="E113" s="139"/>
+      <c r="F113" s="139"/>
+      <c r="G113" s="139"/>
+      <c r="H113" s="139"/>
+      <c r="I113" s="140"/>
       <c r="K113" s="2" t="s">
         <v>41</v>
       </c>
@@ -12719,36 +12866,36 @@
       <c r="N113" s="4"/>
     </row>
     <row r="114" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B114" s="129" t="s">
+      <c r="B114" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C114" s="130"/>
-      <c r="D114" s="130"/>
-      <c r="E114" s="131"/>
-      <c r="F114" s="130" t="s">
+      <c r="C114" s="132"/>
+      <c r="D114" s="132"/>
+      <c r="E114" s="133"/>
+      <c r="F114" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="G114" s="130"/>
-      <c r="H114" s="130"/>
-      <c r="I114" s="131"/>
+      <c r="G114" s="132"/>
+      <c r="H114" s="132"/>
+      <c r="I114" s="133"/>
       <c r="M114" s="4" t="s">
         <v>59</v>
       </c>
       <c r="N114" s="4"/>
     </row>
     <row r="115" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="126" t="s">
+      <c r="B115" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="C115" s="127"/>
-      <c r="D115" s="127"/>
-      <c r="E115" s="128"/>
-      <c r="F115" s="127" t="s">
+      <c r="C115" s="129"/>
+      <c r="D115" s="129"/>
+      <c r="E115" s="130"/>
+      <c r="F115" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="G115" s="127"/>
-      <c r="H115" s="127"/>
-      <c r="I115" s="128"/>
+      <c r="G115" s="129"/>
+      <c r="H115" s="129"/>
+      <c r="I115" s="130"/>
       <c r="K115" s="2" t="s">
         <v>42</v>
       </c>
@@ -13663,7 +13810,7 @@
   </sheetPr>
   <dimension ref="A1:AN121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -13721,235 +13868,235 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:40" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="147" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="147"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="149"/>
       <c r="F2" s="21"/>
-      <c r="G2" s="148" t="s">
+      <c r="G2" s="150" t="s">
         <v>274</v>
       </c>
-      <c r="H2" s="149"/>
-      <c r="I2" s="148" t="s">
+      <c r="H2" s="151"/>
+      <c r="I2" s="150" t="s">
         <v>275</v>
       </c>
-      <c r="J2" s="149"/>
-      <c r="K2" s="148" t="s">
+      <c r="J2" s="151"/>
+      <c r="K2" s="150" t="s">
         <v>276</v>
       </c>
-      <c r="L2" s="149"/>
-      <c r="M2" s="148" t="s">
+      <c r="L2" s="151"/>
+      <c r="M2" s="150" t="s">
         <v>287</v>
       </c>
-      <c r="N2" s="149"/>
-      <c r="O2" s="148" t="s">
+      <c r="N2" s="151"/>
+      <c r="O2" s="150" t="s">
         <v>288</v>
       </c>
-      <c r="P2" s="149"/>
-      <c r="Q2" s="148" t="s">
+      <c r="P2" s="151"/>
+      <c r="Q2" s="150" t="s">
         <v>277</v>
       </c>
-      <c r="R2" s="149"/>
-      <c r="S2" s="148" t="s">
+      <c r="R2" s="151"/>
+      <c r="S2" s="150" t="s">
         <v>278</v>
       </c>
-      <c r="T2" s="149"/>
-      <c r="U2" s="148" t="s">
+      <c r="T2" s="151"/>
+      <c r="U2" s="150" t="s">
         <v>279</v>
       </c>
-      <c r="V2" s="149"/>
-      <c r="W2" s="148" t="s">
+      <c r="V2" s="151"/>
+      <c r="W2" s="150" t="s">
         <v>280</v>
       </c>
-      <c r="X2" s="149"/>
-      <c r="Y2" s="148" t="s">
+      <c r="X2" s="151"/>
+      <c r="Y2" s="150" t="s">
         <v>281</v>
       </c>
-      <c r="Z2" s="149"/>
-      <c r="AA2" s="148" t="s">
+      <c r="Z2" s="151"/>
+      <c r="AA2" s="150" t="s">
         <v>282</v>
       </c>
-      <c r="AB2" s="149"/>
-      <c r="AC2" s="148" t="s">
+      <c r="AB2" s="151"/>
+      <c r="AC2" s="150" t="s">
         <v>283</v>
       </c>
-      <c r="AD2" s="149"/>
-      <c r="AE2" s="148" t="s">
+      <c r="AD2" s="151"/>
+      <c r="AE2" s="150" t="s">
         <v>284</v>
       </c>
-      <c r="AF2" s="149"/>
-      <c r="AG2" s="148" t="s">
+      <c r="AF2" s="151"/>
+      <c r="AG2" s="150" t="s">
         <v>289</v>
       </c>
-      <c r="AH2" s="149"/>
-      <c r="AI2" s="148" t="s">
+      <c r="AH2" s="151"/>
+      <c r="AI2" s="150" t="s">
         <v>290</v>
       </c>
-      <c r="AJ2" s="149"/>
-      <c r="AK2" s="148" t="s">
+      <c r="AJ2" s="151"/>
+      <c r="AK2" s="150" t="s">
         <v>285</v>
       </c>
-      <c r="AL2" s="149"/>
-      <c r="AM2" s="148" t="s">
+      <c r="AL2" s="151"/>
+      <c r="AM2" s="150" t="s">
         <v>286</v>
       </c>
-      <c r="AN2" s="152"/>
+      <c r="AN2" s="154"/>
     </row>
     <row r="3" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="141"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="143"/>
       <c r="F3" s="21"/>
-      <c r="G3" s="129" t="s">
+      <c r="G3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="H3" s="131" t="s">
+      <c r="H3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="I3" s="129" t="s">
+      <c r="I3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="J3" s="131" t="s">
+      <c r="J3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="K3" s="129" t="s">
+      <c r="K3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="L3" s="131" t="s">
+      <c r="L3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="M3" s="129" t="s">
+      <c r="M3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="N3" s="131" t="s">
+      <c r="N3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="O3" s="129" t="s">
+      <c r="O3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="P3" s="131" t="s">
+      <c r="P3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="Q3" s="129" t="s">
+      <c r="Q3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="R3" s="131" t="s">
+      <c r="R3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="S3" s="129" t="s">
+      <c r="S3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="T3" s="131" t="s">
+      <c r="T3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="U3" s="129" t="s">
+      <c r="U3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="V3" s="131" t="s">
+      <c r="V3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="W3" s="129" t="s">
+      <c r="W3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="X3" s="131" t="s">
+      <c r="X3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="Y3" s="129" t="s">
+      <c r="Y3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="Z3" s="131" t="s">
+      <c r="Z3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="AA3" s="129" t="s">
+      <c r="AA3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="AB3" s="131" t="s">
+      <c r="AB3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="AC3" s="129" t="s">
+      <c r="AC3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="AD3" s="131" t="s">
+      <c r="AD3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="AE3" s="129" t="s">
+      <c r="AE3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="AF3" s="131" t="s">
+      <c r="AF3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="AG3" s="129" t="s">
+      <c r="AG3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="AH3" s="131" t="s">
+      <c r="AH3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="AI3" s="129" t="s">
+      <c r="AI3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="AJ3" s="131" t="s">
+      <c r="AJ3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="AK3" s="129" t="s">
+      <c r="AK3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="AL3" s="131" t="s">
+      <c r="AL3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="AM3" s="129" t="s">
+      <c r="AM3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="AN3" s="131" t="s">
+      <c r="AN3" s="133" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:40" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="142" t="s">
+      <c r="B4" s="144" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="144"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="146"/>
       <c r="F4" s="22"/>
-      <c r="G4" s="150"/>
-      <c r="H4" s="151"/>
-      <c r="I4" s="150"/>
-      <c r="J4" s="151"/>
-      <c r="K4" s="150"/>
-      <c r="L4" s="151"/>
-      <c r="M4" s="150"/>
-      <c r="N4" s="151"/>
-      <c r="O4" s="150"/>
-      <c r="P4" s="151"/>
-      <c r="Q4" s="150"/>
-      <c r="R4" s="151"/>
-      <c r="S4" s="150"/>
-      <c r="T4" s="151"/>
-      <c r="U4" s="150"/>
-      <c r="V4" s="151"/>
-      <c r="W4" s="150"/>
-      <c r="X4" s="151"/>
-      <c r="Y4" s="150"/>
-      <c r="Z4" s="151"/>
-      <c r="AA4" s="150"/>
-      <c r="AB4" s="151"/>
-      <c r="AC4" s="150"/>
-      <c r="AD4" s="151"/>
-      <c r="AE4" s="150"/>
-      <c r="AF4" s="151"/>
-      <c r="AG4" s="150"/>
-      <c r="AH4" s="151"/>
-      <c r="AI4" s="150"/>
-      <c r="AJ4" s="151"/>
-      <c r="AK4" s="150"/>
-      <c r="AL4" s="151"/>
-      <c r="AM4" s="150"/>
-      <c r="AN4" s="151"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="153"/>
+      <c r="K4" s="152"/>
+      <c r="L4" s="153"/>
+      <c r="M4" s="152"/>
+      <c r="N4" s="153"/>
+      <c r="O4" s="152"/>
+      <c r="P4" s="153"/>
+      <c r="Q4" s="152"/>
+      <c r="R4" s="153"/>
+      <c r="S4" s="152"/>
+      <c r="T4" s="153"/>
+      <c r="U4" s="152"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="152"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="152"/>
+      <c r="Z4" s="153"/>
+      <c r="AA4" s="152"/>
+      <c r="AB4" s="153"/>
+      <c r="AC4" s="152"/>
+      <c r="AD4" s="153"/>
+      <c r="AE4" s="152"/>
+      <c r="AF4" s="153"/>
+      <c r="AG4" s="152"/>
+      <c r="AH4" s="153"/>
+      <c r="AI4" s="152"/>
+      <c r="AJ4" s="153"/>
+      <c r="AK4" s="152"/>
+      <c r="AL4" s="153"/>
+      <c r="AM4" s="152"/>
+      <c r="AN4" s="153"/>
     </row>
     <row r="5" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
@@ -14776,11 +14923,11 @@
       <c r="T18" s="16"/>
       <c r="U18" s="16"/>
       <c r="V18" s="16"/>
-      <c r="W18" s="153" t="s">
-        <v>1122</v>
-      </c>
-      <c r="X18" s="153" t="s">
+      <c r="W18" s="126" t="s">
         <v>1121</v>
+      </c>
+      <c r="X18" s="126" t="s">
+        <v>1120</v>
       </c>
       <c r="Y18" s="16"/>
       <c r="Z18" s="16"/>
@@ -16900,12 +17047,12 @@
       <c r="AM52" s="16"/>
     </row>
     <row r="53" spans="2:39" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="145" t="s">
+      <c r="B53" s="147" t="s">
         <v>155</v>
       </c>
-      <c r="C53" s="146"/>
-      <c r="D53" s="146"/>
-      <c r="E53" s="147"/>
+      <c r="C53" s="148"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="149"/>
       <c r="F53" s="8"/>
       <c r="G53" s="16"/>
       <c r="H53" s="16"/>
@@ -16939,12 +17086,12 @@
       <c r="AM53" s="16"/>
     </row>
     <row r="54" spans="2:39" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="139" t="s">
+      <c r="B54" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="140"/>
-      <c r="D54" s="140"/>
-      <c r="E54" s="141"/>
+      <c r="C54" s="142"/>
+      <c r="D54" s="142"/>
+      <c r="E54" s="143"/>
       <c r="F54" s="21"/>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
@@ -16976,12 +17123,12 @@
       <c r="AM54" s="16"/>
     </row>
     <row r="55" spans="2:39" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="142" t="s">
+      <c r="B55" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="C55" s="143"/>
-      <c r="D55" s="143"/>
-      <c r="E55" s="144"/>
+      <c r="C55" s="145"/>
+      <c r="D55" s="145"/>
+      <c r="E55" s="146"/>
       <c r="F55" s="22"/>
       <c r="G55" s="16"/>
       <c r="H55" s="16"/>
@@ -20174,7 +20321,7 @@
   <dimension ref="A1:H161"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20197,32 +20344,32 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="147" t="s">
         <v>460</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="147"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="149"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="141"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="143"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="142" t="s">
+      <c r="B4" s="144" t="s">
         <v>461</v>
       </c>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="144"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="146"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -20769,17 +20916,17 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="123" t="s">
         <v>207</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>469</v>
+      <c r="D40" s="124" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E40" s="125" t="s">
+        <v>1123</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -21441,32 +21588,32 @@
     </row>
     <row r="84" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
-      <c r="B84" s="145" t="s">
+      <c r="B84" s="147" t="s">
         <v>460</v>
       </c>
-      <c r="C84" s="146"/>
-      <c r="D84" s="146"/>
-      <c r="E84" s="147"/>
+      <c r="C84" s="148"/>
+      <c r="D84" s="148"/>
+      <c r="E84" s="149"/>
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="B85" s="139" t="s">
+      <c r="B85" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="140"/>
-      <c r="D85" s="140"/>
-      <c r="E85" s="141"/>
+      <c r="C85" s="142"/>
+      <c r="D85" s="142"/>
+      <c r="E85" s="143"/>
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
-      <c r="B86" s="142" t="s">
+      <c r="B86" s="144" t="s">
         <v>462</v>
       </c>
-      <c r="C86" s="143"/>
-      <c r="D86" s="143"/>
-      <c r="E86" s="144"/>
+      <c r="C86" s="145"/>
+      <c r="D86" s="145"/>
+      <c r="E86" s="146"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -22580,7 +22727,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" topLeftCell="A31">
-      <selection activeCell="K50" sqref="K50"/>
+      <selection activeCell="J49" sqref="J49"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="4294967295" r:id="rId1"/>
     </customSheetView>
@@ -22638,54 +22785,54 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="147" t="s">
         <v>530</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="147"/>
-      <c r="G2" s="148" t="s">
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="149"/>
+      <c r="G2" s="150" t="s">
         <v>537</v>
       </c>
-      <c r="H2" s="152"/>
-      <c r="J2" s="148" t="s">
+      <c r="H2" s="154"/>
+      <c r="J2" s="150" t="s">
         <v>538</v>
       </c>
-      <c r="K2" s="152"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="141"/>
-      <c r="G3" s="129" t="s">
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="143"/>
+      <c r="G3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="H3" s="131" t="s">
+      <c r="H3" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="J3" s="129" t="s">
+      <c r="J3" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="K3" s="131" t="s">
+      <c r="K3" s="133" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="142" t="s">
+      <c r="B4" s="144" t="s">
         <v>531</v>
       </c>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="144"/>
-      <c r="G4" s="150"/>
-      <c r="H4" s="151"/>
-      <c r="J4" s="150"/>
-      <c r="K4" s="151"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="146"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="153"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="153"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -23113,30 +23260,30 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="147" t="s">
         <v>530</v>
       </c>
-      <c r="C25" s="146"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="147"/>
+      <c r="C25" s="148"/>
+      <c r="D25" s="148"/>
+      <c r="E25" s="149"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="139" t="s">
+      <c r="B26" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="140"/>
-      <c r="D26" s="140"/>
-      <c r="E26" s="141"/>
+      <c r="C26" s="142"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="143"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="142" t="s">
+      <c r="B27" s="144" t="s">
         <v>536</v>
       </c>
-      <c r="C27" s="143"/>
-      <c r="D27" s="143"/>
-      <c r="E27" s="144"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="146"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -23636,31 +23783,31 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="147" t="s">
         <v>740</v>
       </c>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="147"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="141" t="s">
         <v>741</v>
       </c>
-      <c r="B3" s="140"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="141"/>
+      <c r="B3" s="142"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="143"/>
       <c r="J3" s="53"/>
       <c r="K3" s="53"/>
       <c r="L3" s="53"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="142" t="s">
+      <c r="A4" s="144" t="s">
         <v>742</v>
       </c>
-      <c r="B4" s="143"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="144"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="146"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">

</xml_diff>